<commit_message>
Fix evaluation and API KEY
</commit_message>
<xml_diff>
--- a/results/mistral_evaluation_stg1.xlsx
+++ b/results/mistral_evaluation_stg1.xlsx
@@ -482,7 +482,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ToT Prompt</t>
+          <t>Prompt ToT</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -501,7 +501,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ToT Graph</t>
+          <t>Graph ToT</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -520,7 +520,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Optimization</t>
+          <t>Optimized</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>